<commit_message>
replace some occurences of BJ-DIANE with TROY-DIANE
git-svn-id: file://localhost/tmp/svn2git/svn@5218 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/perf/data.xlsx
+++ b/papers/troy/pstar/perf/data.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21105"/>
-  <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr date1904="1" showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="36020" windowHeight="28360" tabRatio="500" activeTab="1"/>
   </bookViews>
@@ -10,9 +10,9 @@
     <sheet name="data.csv" sheetId="1" r:id="rId1"/>
     <sheet name="Blatt3" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="11" r:id="rId3"/>
+    <pivotCache cacheId="12" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -78,7 +78,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -122,7 +122,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -136,31 +136,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <alignment vertical="center"/>
     </dxf>
@@ -394,11 +370,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="601690184"/>
-        <c:axId val="680613048"/>
+        <c:axId val="601836312"/>
+        <c:axId val="597797240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="601690184"/>
+        <c:axId val="601836312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -434,7 +410,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="680613048"/>
+        <c:crossAx val="597797240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -442,7 +418,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="680613048"/>
+        <c:axId val="597797240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -472,7 +448,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="601690184"/>
+        <c:crossAx val="601836312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -544,10 +520,10 @@
     <cacheField name="#jobs" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="16" maxValue="512"/>
     </cacheField>
-    <cacheField name="Runtime" numFmtId="170">
+    <cacheField name="Runtime" numFmtId="164">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="6.6093559265100001" maxValue="2927.9610979600002"/>
     </cacheField>
-    <cacheField name="Queuing Time" numFmtId="170">
+    <cacheField name="Queuing Time" numFmtId="164">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.18493008613600001" maxValue="96.081320047399998"/>
     </cacheField>
     <cacheField name="Coordination URL" numFmtId="0">
@@ -564,7 +540,7 @@
     <cacheField name="Subjob Submission Time" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.15921211242700001" maxValue="1868.77072692"/>
     </cacheField>
-    <cacheField name="Jobs/sec" numFmtId="170">
+    <cacheField name="Jobs/sec" numFmtId="164">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.17086182360087668" maxValue="22.584690874685425"/>
     </cacheField>
     <cacheField name="Total cores" numFmtId="0">
@@ -1554,14 +1530,14 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" outline="1" outlineData="1" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" outline="1" outlineData="1" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:E9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField compact="0" showAll="0"/>
     <pivotField compact="0" showAll="0"/>
     <pivotField compact="0" showAll="0"/>
-    <pivotField dataField="1" compact="0" numFmtId="170" showAll="0"/>
-    <pivotField compact="0" numFmtId="170" showAll="0"/>
+    <pivotField dataField="1" compact="0" numFmtId="164" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" showAll="0"/>
     <pivotField axis="axisCol" compact="0" showAll="0">
       <items count="5">
         <item x="2"/>
@@ -1573,7 +1549,7 @@
     </pivotField>
     <pivotField compact="0" showAll="0"/>
     <pivotField compact="0" showAll="0"/>
-    <pivotField compact="0" numFmtId="170" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" showAll="0"/>
     <pivotField axis="axisRow" compact="0" showAll="0">
       <items count="9">
         <item m="1" x="6"/>
@@ -1966,8 +1942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E46" sqref="E32:E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4642,7 +4618,7 @@
   <dimension ref="A3:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I66" sqref="I66"/>
+      <selection activeCell="E5" sqref="E5:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4650,7 +4626,8 @@
     <col min="1" max="1" width="18.83203125" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" customWidth="1"/>
     <col min="3" max="3" width="25.6640625" customWidth="1"/>
-    <col min="4" max="5" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" customWidth="1"/>
     <col min="6" max="13" width="27.6640625" customWidth="1"/>
     <col min="14" max="44" width="12.1640625" customWidth="1"/>
     <col min="45" max="45" width="11.1640625" customWidth="1"/>

</xml_diff>